<commit_message>
script to pull NLDAS met data and subfolder structure for data
</commit_message>
<xml_diff>
--- a/Teleconnections/Lake_Characteristics.xlsx
+++ b/Teleconnections/Lake_Characteristics.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3416" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="92">
   <si>
     <t>Crampton Lake</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>Toolik Environmental Data Center</t>
+  </si>
+  <si>
+    <t>Prairie Lake</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1005,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1430,6 +1433,20 @@
       </c>
       <c r="M10" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3">
+        <v>47.159408999999997</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-99.117631000000003</v>
       </c>
     </row>
     <row r="17" spans="13:13" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
first cut Prairie Pothole GLM
</commit_message>
<xml_diff>
--- a/Teleconnections/Lake_Characteristics.xlsx
+++ b/Teleconnections/Lake_Characteristics.xlsx
@@ -17,10 +17,10 @@
     <sheet name="Barco" sheetId="2" r:id="rId3"/>
     <sheet name="Crampton" sheetId="9" r:id="rId4"/>
     <sheet name="Mendota" sheetId="3" r:id="rId5"/>
-    <sheet name="FallingCreek" sheetId="7" r:id="rId6"/>
+    <sheet name="Falling Creek" sheetId="7" r:id="rId6"/>
     <sheet name="Little Rock" sheetId="12" r:id="rId7"/>
     <sheet name="Prairie" sheetId="10" r:id="rId8"/>
-    <sheet name="PrPothole" sheetId="11" r:id="rId9"/>
+    <sheet name="Prairie Pothole" sheetId="11" r:id="rId9"/>
     <sheet name="Suggs" sheetId="6" r:id="rId10"/>
     <sheet name="Sunapee" sheetId="4" r:id="rId11"/>
     <sheet name="Toolik" sheetId="8" r:id="rId12"/>
@@ -1004,9 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6899,7 +6897,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40:B69"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21726,7 +21724,7 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update Lake Characteristics lat/long precision
</commit_message>
<xml_diff>
--- a/Teleconnections/Lake_Characteristics.xlsx
+++ b/Teleconnections/Lake_Characteristics.xlsx
@@ -304,6 +304,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -454,7 +457,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -488,6 +491,10 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -859,8 +866,8 @@
   <cols>
     <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.75" style="1" bestFit="1" customWidth="1"/>
@@ -879,10 +886,10 @@
       <c r="B1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="14" t="s">
@@ -920,11 +927,11 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
-        <v>29.676469999999998</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-82.00909</v>
+      <c r="C2" s="18">
+        <v>29.675940000000001</v>
+      </c>
+      <c r="D2" s="18">
+        <v>-82.008229999999998</v>
       </c>
       <c r="E2">
         <v>28</v>
@@ -961,11 +968,11 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
-        <v>46.211109999999998</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-89.478250000000003</v>
+      <c r="C3" s="18">
+        <v>46.210250000000002</v>
+      </c>
+      <c r="D3" s="18">
+        <v>-89.47345</v>
       </c>
       <c r="E3">
         <v>591</v>
@@ -1002,10 +1009,10 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="18">
         <v>37.303330000000003</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="18">
         <v>-79.837221999999997</v>
       </c>
       <c r="E4">
@@ -1043,10 +1050,10 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="18">
         <v>43.109699999999997</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="18">
         <v>-89.420599999999993</v>
       </c>
       <c r="E5">
@@ -1084,10 +1091,10 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="18">
         <v>43.380200000000002</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="18">
         <v>-72.052700000000002</v>
       </c>
       <c r="E6">
@@ -1125,11 +1132,11 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>47.129989999999999</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-99.250550000000004</v>
+      <c r="C7" s="18">
+        <v>47.130119999999998</v>
+      </c>
+      <c r="D7" s="18">
+        <v>-99.253020000000006</v>
       </c>
       <c r="E7">
         <v>565</v>
@@ -1166,11 +1173,11 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
-        <v>29.687049999999999</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-82.016170000000002</v>
+      <c r="C8" s="18">
+        <v>29.6877</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-82.017849999999996</v>
       </c>
       <c r="E8">
         <v>29</v>
@@ -1207,10 +1214,10 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="18">
         <v>68.629559999999998</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="18">
         <v>-149.61051</v>
       </c>
       <c r="E9">
@@ -1274,7 +1281,7 @@
     <col min="6" max="6" width="28.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>46</v>
       </c>

</xml_diff>